<commit_message>
chỉnh sửa cấu trúc hàm getProgramCreateSchedule và sửa lỗi syntax của python
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK2_CT01_2025/LichHocKy_HK2_CT01_2025.xlsx
+++ b/timetabling_GA/results/HK2_CT01_2025/LichHocKy_HK2_CT01_2025.xlsx
@@ -85,18 +85,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00BDD7EE"/>
+        <bgColor rgb="00BDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFCCCB"/>
         <bgColor rgb="00FFCCCB"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,44 +118,11 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -181,7 +148,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -550,7 +516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,16 +626,16 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
@@ -678,74 +644,19 @@
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="8" t="inlineStr">
         <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
-        <is>
           <t>MH004
 (Theory)
 Room: LT3
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -880,12 +791,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -893,32 +829,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -942,15 +853,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -1092,12 +1003,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -1105,32 +1041,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -1154,15 +1065,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -1304,12 +1215,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -1317,32 +1253,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -1366,15 +1277,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -1516,12 +1427,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -1529,32 +1465,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -1578,15 +1489,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -1728,12 +1639,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -1741,32 +1677,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -1790,15 +1701,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -1940,12 +1851,37 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -1953,32 +1889,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -2002,15 +1913,15 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11"/>
@@ -2031,7 +1942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2141,20 +2052,18 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="10" t="inlineStr">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>MH003
 (Theory)
@@ -2162,12 +2071,43 @@
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
-    <row r="9"/>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -2185,7 +2125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2300,18 +2240,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -2319,24 +2283,7 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -2344,24 +2291,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -2369,14 +2299,35 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -2397,42 +2348,8 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -2440,19 +2357,23 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -2466,7 +2387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2581,18 +2502,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -2600,24 +2545,7 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -2625,24 +2553,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -2650,14 +2561,35 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -2678,42 +2610,8 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -2721,19 +2619,23 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -2747,7 +2649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2862,18 +2764,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -2881,24 +2807,7 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -2906,24 +2815,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -2931,14 +2823,35 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -2959,42 +2872,8 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -3002,19 +2881,23 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3028,7 +2911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3143,18 +3026,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -3162,24 +3069,7 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -3187,24 +3077,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -3212,14 +3085,35 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -3240,42 +3134,8 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -3283,19 +3143,23 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3309,7 +3173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3424,18 +3288,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -3443,24 +3331,7 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -3468,24 +3339,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -3493,14 +3347,35 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -3521,42 +3396,8 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>MH004
 (Practice)
@@ -3564,19 +3405,23 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3705,18 +3550,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -3724,31 +3593,18 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
-        <is>
-          <t>MH004
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -3759,22 +3615,22 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -3795,33 +3651,25 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3950,18 +3798,42 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -3969,31 +3841,18 @@
 Lecturer: GV007</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="10" t="inlineStr">
-        <is>
-          <t>MH004
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -4004,22 +3863,22 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
-(Theory)
-Room: LT2
+(Practice)
+Room: TH2
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
@@ -4040,33 +3899,25 @@
         <v>35</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Practice)
-Room: TH2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -4080,7 +3931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4201,12 +4052,44 @@
       <c r="C8" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Practice)
+Room: TH2
+Lecturer: GV007</t>
+        </is>
+      </c>
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>MH004
 (Theory)
@@ -4214,32 +4097,7 @@
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
@@ -4248,7 +4106,7 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -4260,7 +4118,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Practice)
@@ -4270,18 +4128,40 @@
       </c>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="10" t="inlineStr">
-        <is>
-          <t>MH003
-(Theory)
-Room: LT1
-Lecturer: GV007</t>
-        </is>
-      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
-    <row r="11"/>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Theory)
+Room: LT3
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>

</xml_diff>